<commit_message>
finished CSG1132 week 5 lab
</commit_message>
<xml_diff>
--- a/year_1/sem_1/CSG1132_communicating_in_an_it_environment/05_week_5/csg1132-1-2013-Ass2-dataset-inclass-exercise.xlsx
+++ b/year_1/sem_1/CSG1132_communicating_in_an_it_environment/05_week_5/csg1132-1-2013-Ass2-dataset-inclass-exercise.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marty\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marty\Dropbox\Documents\ecu\year_1\sem_1\CSG1132_communicating_in_an_it_environment\05_week_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29145" windowHeight="12630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29145" windowHeight="12630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FB" sheetId="1" r:id="rId1"/>
-    <sheet name="NORMAL DISTRIBUTION" sheetId="4" r:id="rId2"/>
-    <sheet name="Explanation" sheetId="3" r:id="rId3"/>
+    <sheet name="ND1 Hours" sheetId="5" r:id="rId2"/>
+    <sheet name="ND2 Hours" sheetId="6" r:id="rId3"/>
+    <sheet name="Explanation" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Att_to_privacy">Explanation!$A$4</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Age</t>
   </si>
@@ -107,9 +108,6 @@
     <t>Your status as an intravert or extravert</t>
   </si>
   <si>
-    <t>Bins</t>
-  </si>
-  <si>
     <t>Bin</t>
   </si>
   <si>
@@ -119,14 +117,29 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>CORRELATION</t>
+    <t>Lower Interval</t>
+  </si>
+  <si>
+    <t>Upper Interval</t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Interval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +228,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -290,7 +311,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -392,11 +413,17 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -468,9 +495,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'NORMAL DISTRIBUTION'!$G$3:$G$20</c:f>
+              <c:f>'ND1 Hours'!$D$2:$D$36</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -523,6 +550,57 @@
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>More</c:v>
                 </c:pt>
               </c:strCache>
@@ -530,10 +608,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'NORMAL DISTRIBUTION'!$H$3:$H$20</c:f>
+              <c:f>'ND1 Hours'!$E$2:$E$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -586,6 +664,57 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -601,11 +730,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="291441728"/>
-        <c:axId val="291442288"/>
+        <c:axId val="230791392"/>
+        <c:axId val="232475264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="291441728"/>
+        <c:axId val="230791392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,7 +763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291442288"/>
+        <c:crossAx val="232475264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -642,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291442288"/>
+        <c:axId val="232475264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291441728"/>
+        <c:crossAx val="230791392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -693,24 +822,1008 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ND2 Hours'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frequency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'ND2 Hours'!$F$2:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ND2 Hours'!$G$2:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="229832304"/>
+        <c:axId val="230719824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="229832304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="230719824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="230719824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="229832304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1015,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1034,7 +2147,7 @@
     <col min="10" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +2162,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="2:13" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +2188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21">
         <v>26</v>
       </c>
@@ -1100,15 +2213,8 @@
       <c r="I3" s="22">
         <v>12</v>
       </c>
-      <c r="L3" s="22">
-        <f>CORREL(E3:E64,I3:I64)</f>
-        <v>3.2813364366773297E-2</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="21">
         <v>18</v>
       </c>
@@ -1133,12 +2239,8 @@
       <c r="I4" s="22">
         <v>12</v>
       </c>
-      <c r="L4" s="22">
-        <f>CORREL(F3:F64,I3:I64)</f>
-        <v>0.86000103954853135</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21">
         <v>20</v>
       </c>
@@ -1164,7 +2266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="21">
         <v>20</v>
       </c>
@@ -1190,7 +2292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21">
         <v>21</v>
       </c>
@@ -1216,7 +2318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="21">
         <v>19</v>
       </c>
@@ -1242,7 +2344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="21">
         <v>20</v>
       </c>
@@ -1268,7 +2370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
         <v>18</v>
       </c>
@@ -1294,7 +2396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
         <v>17</v>
       </c>
@@ -1320,7 +2422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
         <v>27</v>
       </c>
@@ -1346,7 +2448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21">
         <v>27</v>
       </c>
@@ -1372,7 +2474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21">
         <v>18</v>
       </c>
@@ -1398,7 +2500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21">
         <v>19</v>
       </c>
@@ -1424,7 +2526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:13" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21">
         <v>17</v>
       </c>
@@ -2692,84 +3794,281 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H65" s="24"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G66" s="22"/>
       <c r="H66" s="22"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="17">
-        <f>AVERAGE(B3:B64)</f>
+        <f t="shared" ref="B67:I67" si="0">AVERAGE(B3:B64)</f>
         <v>20.774193548387096</v>
       </c>
+      <c r="C67" s="18">
+        <f t="shared" si="0"/>
+        <v>0.95081967213114749</v>
+      </c>
+      <c r="D67" s="18">
+        <f t="shared" si="0"/>
+        <v>12.262295081967213</v>
+      </c>
       <c r="E67" s="18">
-        <f>AVERAGE(E3:E64)</f>
+        <f t="shared" si="0"/>
         <v>15.344262295081966</v>
       </c>
-      <c r="H67" s="25"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F67" s="18">
+        <f t="shared" si="0"/>
+        <v>270.22033898305085</v>
+      </c>
+      <c r="G67" s="18">
+        <f t="shared" si="0"/>
+        <v>22.70967741935484</v>
+      </c>
+      <c r="H67" s="25">
+        <f t="shared" si="0"/>
+        <v>3.5806451612903225</v>
+      </c>
+      <c r="I67" s="18">
+        <f t="shared" si="0"/>
+        <v>13.016129032258064</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F68" s="33"/>
-      <c r="G68" s="33"/>
-      <c r="H68" s="36"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="17">
+        <f t="shared" ref="B68:I68" si="1">MEDIAN(B3:B64)</f>
+        <v>19.5</v>
+      </c>
+      <c r="C68" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D68" s="18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E68" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F68" s="33">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="G68" s="33">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H68" s="36">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I68" s="18">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F69" s="33"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="17">
+        <f t="shared" ref="B69:I69" si="2">MODE(B3:B64)</f>
+        <v>19</v>
+      </c>
+      <c r="C69" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E69" s="18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F69" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="32">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="H69" s="32">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="I69" s="18">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G70" s="33"/>
-      <c r="H70" s="33"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B70" s="17">
+        <f t="shared" ref="B70:I70" si="3">_xlfn.STDEV.S(B3:B64)</f>
+        <v>3.0751215081348859</v>
+      </c>
+      <c r="C70" s="18">
+        <f t="shared" si="3"/>
+        <v>0.21803894974650131</v>
+      </c>
+      <c r="D70" s="18">
+        <f t="shared" si="3"/>
+        <v>12.239147082680043</v>
+      </c>
+      <c r="E70" s="18">
+        <f t="shared" si="3"/>
+        <v>25.237462396142789</v>
+      </c>
+      <c r="F70" s="18">
+        <f t="shared" si="3"/>
+        <v>177.78872271328416</v>
+      </c>
+      <c r="G70" s="33">
+        <f t="shared" si="3"/>
+        <v>15.852172728749352</v>
+      </c>
+      <c r="H70" s="33">
+        <f t="shared" si="3"/>
+        <v>0.87867984241588626</v>
+      </c>
+      <c r="I70" s="18">
+        <f t="shared" si="3"/>
+        <v>3.9400920996303559</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="31" t="s">
         <v>7</v>
       </c>
+      <c r="B71" s="17">
+        <f t="shared" ref="B71:I71" si="4">SKEW(B3:B64)</f>
+        <v>0.93990973811448486</v>
+      </c>
+      <c r="C71" s="18">
+        <f t="shared" si="4"/>
+        <v>-4.2753984593776178</v>
+      </c>
+      <c r="D71" s="18">
+        <f t="shared" si="4"/>
+        <v>1.8777002796993696</v>
+      </c>
       <c r="E71" s="18">
-        <f>SKEW(E3:E64)</f>
+        <f t="shared" si="4"/>
         <v>4.3352245156387541</v>
       </c>
-      <c r="G71" s="33"/>
-      <c r="H71" s="33"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F71" s="18">
+        <f t="shared" si="4"/>
+        <v>0.77179046910845805</v>
+      </c>
+      <c r="G71" s="33">
+        <f t="shared" si="4"/>
+        <v>1.7076011014877246</v>
+      </c>
+      <c r="H71" s="33">
+        <f t="shared" si="4"/>
+        <v>-0.70357728519460427</v>
+      </c>
+      <c r="I71" s="18">
+        <f t="shared" si="4"/>
+        <v>0.58910852000334091</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G72" s="33"/>
-      <c r="H72" s="33"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B72" s="17">
+        <f t="shared" ref="B72:I72" si="5">KURT(B3:B64)</f>
+        <v>-9.236819764383819E-2</v>
+      </c>
+      <c r="C72" s="18">
+        <f t="shared" si="5"/>
+        <v>16.830044942461498</v>
+      </c>
+      <c r="D72" s="18">
+        <f t="shared" si="5"/>
+        <v>4.3629867112537646</v>
+      </c>
+      <c r="E72" s="18">
+        <f t="shared" si="5"/>
+        <v>23.344924838643578</v>
+      </c>
+      <c r="F72" s="18">
+        <f t="shared" si="5"/>
+        <v>0.31199068331770929</v>
+      </c>
+      <c r="G72" s="33">
+        <f t="shared" si="5"/>
+        <v>3.5119451870077376</v>
+      </c>
+      <c r="H72" s="33">
+        <f t="shared" si="5"/>
+        <v>0.33995911084535946</v>
+      </c>
+      <c r="I72" s="18">
+        <f t="shared" si="5"/>
+        <v>-4.4933404912368413E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="17">
+        <f t="shared" ref="B73:I73" si="6">MAX(B4:B64)</f>
+        <v>29</v>
+      </c>
+      <c r="C73" s="18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D73" s="18">
+        <f t="shared" si="6"/>
+        <v>59</v>
+      </c>
+      <c r="E73" s="18">
+        <f t="shared" si="6"/>
+        <v>169</v>
+      </c>
+      <c r="F73" s="18">
+        <f t="shared" si="6"/>
+        <v>798</v>
+      </c>
+      <c r="G73" s="33">
+        <f t="shared" si="6"/>
+        <v>83</v>
+      </c>
+      <c r="H73" s="33">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="I73" s="18">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G74" s="33"/>
       <c r="H74" s="33"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G75" s="33"/>
       <c r="H75" s="33"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G76" s="33"/>
       <c r="H76" s="33"/>
     </row>
@@ -2785,502 +4084,1362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D1" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="18">
         <v>5</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="D2" s="38">
+        <v>5</v>
+      </c>
+      <c r="E2" s="39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>5</v>
+      </c>
+      <c r="B3" s="18">
+        <v>10</v>
+      </c>
+      <c r="D3" s="38">
+        <v>10</v>
+      </c>
+      <c r="E3" s="39">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>19</v>
+      </c>
+      <c r="B4" s="18">
+        <v>15</v>
+      </c>
+      <c r="D4" s="38">
+        <v>15</v>
+      </c>
+      <c r="E4" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>31</v>
+      </c>
+      <c r="B5" s="18">
+        <v>20</v>
+      </c>
+      <c r="D5" s="38">
+        <v>20</v>
+      </c>
+      <c r="E5" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>25</v>
       </c>
-      <c r="H2" s="40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B6" s="18">
+        <v>25</v>
+      </c>
+      <c r="D6" s="38">
+        <v>25</v>
+      </c>
+      <c r="E6" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>31</v>
+      </c>
+      <c r="B7" s="18">
+        <v>30</v>
+      </c>
+      <c r="D7" s="38">
+        <v>30</v>
+      </c>
+      <c r="E7" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>26</v>
+      </c>
+      <c r="B8" s="18">
+        <v>35</v>
+      </c>
+      <c r="D8" s="38">
+        <v>35</v>
+      </c>
+      <c r="E8" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="G3" s="37">
+      <c r="B9" s="18">
+        <v>40</v>
+      </c>
+      <c r="D9" s="38">
+        <v>40</v>
+      </c>
+      <c r="E9" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>21</v>
+      </c>
+      <c r="B10" s="18">
+        <v>45</v>
+      </c>
+      <c r="D10" s="38">
+        <v>45</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18">
+        <v>50</v>
+      </c>
+      <c r="D11" s="38">
+        <v>50</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>2</v>
+      </c>
+      <c r="B12" s="18">
+        <v>55</v>
+      </c>
+      <c r="D12" s="38">
+        <v>55</v>
+      </c>
+      <c r="E12" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>8</v>
+      </c>
+      <c r="B13" s="18">
+        <v>60</v>
+      </c>
+      <c r="D13" s="38">
+        <v>60</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="18">
+        <v>65</v>
+      </c>
+      <c r="D14" s="38">
+        <v>65</v>
+      </c>
+      <c r="E14" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>3</v>
+      </c>
+      <c r="B15" s="18">
+        <v>70</v>
+      </c>
+      <c r="D15" s="38">
+        <v>70</v>
+      </c>
+      <c r="E15" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18">
+        <v>75</v>
+      </c>
+      <c r="D16" s="38">
+        <v>75</v>
+      </c>
+      <c r="E16" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>29</v>
+      </c>
+      <c r="B17" s="18">
+        <v>80</v>
+      </c>
+      <c r="D17" s="38">
+        <v>80</v>
+      </c>
+      <c r="E17" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>8</v>
+      </c>
+      <c r="B18" s="18">
+        <v>85</v>
+      </c>
+      <c r="D18" s="38">
+        <v>85</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>8</v>
+      </c>
+      <c r="B19" s="18">
+        <v>90</v>
+      </c>
+      <c r="D19" s="38">
+        <v>90</v>
+      </c>
+      <c r="E19" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>7</v>
+      </c>
+      <c r="B20" s="18">
+        <v>95</v>
+      </c>
+      <c r="D20" s="38">
+        <v>95</v>
+      </c>
+      <c r="E20" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>2</v>
+      </c>
+      <c r="B21" s="18">
+        <v>100</v>
+      </c>
+      <c r="D21" s="38">
+        <v>100</v>
+      </c>
+      <c r="E21" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>11</v>
+      </c>
+      <c r="B22" s="18">
+        <v>105</v>
+      </c>
+      <c r="D22" s="38">
+        <v>105</v>
+      </c>
+      <c r="E22" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>6</v>
+      </c>
+      <c r="B23" s="18">
+        <v>110</v>
+      </c>
+      <c r="D23" s="38">
+        <v>110</v>
+      </c>
+      <c r="E23" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>8</v>
+      </c>
+      <c r="B24" s="18">
+        <v>115</v>
+      </c>
+      <c r="D24" s="38">
+        <v>115</v>
+      </c>
+      <c r="E24" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
         <v>5</v>
       </c>
-      <c r="H3" s="38">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>19</v>
-      </c>
-      <c r="C4">
+      <c r="B25" s="18">
+        <v>120</v>
+      </c>
+      <c r="D25" s="38">
+        <v>120</v>
+      </c>
+      <c r="E25" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>0</v>
+      </c>
+      <c r="B26" s="18">
+        <v>125</v>
+      </c>
+      <c r="D26" s="38">
+        <v>125</v>
+      </c>
+      <c r="E26" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>3</v>
+      </c>
+      <c r="B27" s="18">
+        <v>130</v>
+      </c>
+      <c r="D27" s="38">
+        <v>130</v>
+      </c>
+      <c r="E27" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <v>7</v>
+      </c>
+      <c r="B28" s="18">
+        <v>135</v>
+      </c>
+      <c r="D28" s="38">
+        <v>135</v>
+      </c>
+      <c r="E28" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <v>2</v>
+      </c>
+      <c r="B29" s="18">
+        <v>140</v>
+      </c>
+      <c r="D29" s="38">
+        <v>140</v>
+      </c>
+      <c r="E29" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <v>5</v>
+      </c>
+      <c r="B30" s="18">
+        <v>145</v>
+      </c>
+      <c r="D30" s="38">
+        <v>145</v>
+      </c>
+      <c r="E30" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <v>9</v>
+      </c>
+      <c r="B31" s="18">
+        <v>150</v>
+      </c>
+      <c r="D31" s="38">
+        <v>150</v>
+      </c>
+      <c r="E31" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <v>0</v>
+      </c>
+      <c r="B32" s="18">
+        <v>155</v>
+      </c>
+      <c r="D32" s="38">
+        <v>155</v>
+      </c>
+      <c r="E32" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="21">
+        <v>4</v>
+      </c>
+      <c r="B33" s="18">
+        <v>160</v>
+      </c>
+      <c r="D33" s="38">
+        <v>160</v>
+      </c>
+      <c r="E33" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
         <v>15</v>
       </c>
-      <c r="G4" s="37">
-        <v>10</v>
-      </c>
-      <c r="H4" s="38">
+      <c r="B34" s="18">
+        <v>165</v>
+      </c>
+      <c r="D34" s="38">
+        <v>165</v>
+      </c>
+      <c r="E34" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>6</v>
+      </c>
+      <c r="B35" s="18">
+        <v>170</v>
+      </c>
+      <c r="D35" s="38">
+        <v>170</v>
+      </c>
+      <c r="E35" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23">
+        <v>25</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="D36" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23">
+        <v>3</v>
+      </c>
+      <c r="B37" s="18"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="24">
+        <v>76</v>
+      </c>
+      <c r="B38" s="18"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="24">
+        <v>36</v>
+      </c>
+      <c r="B39" s="18"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
+        <v>53</v>
+      </c>
+      <c r="B40" s="18"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="24">
+        <v>3</v>
+      </c>
+      <c r="B41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="24">
+        <v>4</v>
+      </c>
+      <c r="B42" s="18"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="24">
+        <v>2</v>
+      </c>
+      <c r="B43" s="18"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
+        <v>71</v>
+      </c>
+      <c r="B44" s="18"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="24">
+        <v>4</v>
+      </c>
+      <c r="B45" s="18"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="24">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="G5" s="37">
-        <v>15</v>
-      </c>
-      <c r="H5" s="38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="C6">
-        <v>25</v>
-      </c>
-      <c r="G6" s="37">
-        <v>20</v>
-      </c>
-      <c r="H6" s="38">
+      <c r="B46" s="18"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>31</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="G7" s="37">
-        <v>25</v>
-      </c>
-      <c r="H7" s="38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B47" s="18"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="24">
+        <v>16</v>
+      </c>
+      <c r="B48" s="18"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="24">
+        <v>0</v>
+      </c>
+      <c r="B49" s="18"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="24">
+        <v>8</v>
+      </c>
+      <c r="B50" s="18"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="24">
+        <v>8</v>
+      </c>
+      <c r="B51" s="18"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="24">
+        <v>8</v>
+      </c>
+      <c r="B52" s="18"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="24">
+        <v>22</v>
+      </c>
+      <c r="B53" s="18"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="24">
         <v>26</v>
       </c>
-      <c r="C8">
-        <v>35</v>
-      </c>
-      <c r="G8" s="37">
-        <v>30</v>
-      </c>
-      <c r="H8" s="38">
+      <c r="B54" s="18"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="24">
+        <v>7</v>
+      </c>
+      <c r="B55" s="18"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="24">
+        <v>5</v>
+      </c>
+      <c r="B56" s="18"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="G9" s="37">
-        <v>35</v>
-      </c>
-      <c r="H9" s="38">
+      <c r="B57" s="18"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="24">
+        <v>7</v>
+      </c>
+      <c r="B58" s="18"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="24">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>45</v>
-      </c>
-      <c r="G10" s="37">
-        <v>40</v>
-      </c>
-      <c r="H10" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="G11" s="37">
-        <v>45</v>
-      </c>
-      <c r="H11" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>55</v>
-      </c>
-      <c r="G12" s="37">
-        <v>50</v>
-      </c>
-      <c r="H12" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>60</v>
-      </c>
-      <c r="G13" s="37">
-        <v>55</v>
-      </c>
-      <c r="H13" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>65</v>
-      </c>
-      <c r="G14" s="37">
-        <v>60</v>
-      </c>
-      <c r="H14" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>70</v>
-      </c>
-      <c r="G15" s="37">
-        <v>65</v>
-      </c>
-      <c r="H15" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>75</v>
-      </c>
-      <c r="G16" s="37">
-        <v>70</v>
-      </c>
-      <c r="H16" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>29</v>
-      </c>
-      <c r="C17">
-        <v>80</v>
-      </c>
-      <c r="G17" s="37">
-        <v>75</v>
-      </c>
-      <c r="H17" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>85</v>
-      </c>
-      <c r="G18" s="37">
-        <v>80</v>
-      </c>
-      <c r="H18" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="G19" s="37">
-        <v>85</v>
-      </c>
-      <c r="H19" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="G20" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B59" s="18"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="24">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B60" s="18"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="24">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>6</v>
-      </c>
+      <c r="B61" s="18"/>
     </row>
   </sheetData>
-  <sortState ref="G3:G19">
-    <sortCondition ref="G3"/>
+  <sortState ref="D2:D35">
+    <sortCondition ref="D2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
+        <v>15</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="21">
+        <f>MAX(A2:A61)</f>
+        <v>76</v>
+      </c>
+      <c r="D2" s="18">
+        <v>0</v>
+      </c>
+      <c r="E2" s="18">
+        <f>D2 + 7.6</f>
+        <v>7.6</v>
+      </c>
+      <c r="F2" s="18">
+        <v>4</v>
+      </c>
+      <c r="G2" s="18">
+        <f t="array" ref="G2:G20">FREQUENCY(A2:A61,F2:F20)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <v>5</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="21">
+        <f>MIN(A2:A61)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="18">
+        <f>E2 + 1</f>
+        <v>8.6</v>
+      </c>
+      <c r="E3" s="18">
+        <f>E2 + 7.6</f>
+        <v>15.2</v>
+      </c>
+      <c r="F3" s="18">
+        <v>8</v>
+      </c>
+      <c r="G3" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <v>19</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="21">
+        <f>C2-C3</f>
+        <v>76</v>
+      </c>
+      <c r="D4" s="18">
+        <f t="shared" ref="D4:D16" si="0">E3 + 1</f>
+        <v>16.2</v>
+      </c>
+      <c r="E4" s="18">
+        <f t="shared" ref="E4:E16" si="1">E3 + 7.6</f>
+        <v>22.799999999999997</v>
+      </c>
+      <c r="F4" s="18">
+        <v>12</v>
+      </c>
+      <c r="G4" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <v>31</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="21">
+        <f>C4 / 10</f>
+        <v>7.6</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" si="0"/>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="E5" s="18">
+        <f t="shared" si="1"/>
+        <v>30.4</v>
+      </c>
+      <c r="F5" s="18">
+        <v>16</v>
+      </c>
+      <c r="G5" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <v>25</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="21">
+        <f>AVERAGE(A2:A61)</f>
+        <v>12.783333333333333</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" si="0"/>
+        <v>31.4</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="F6" s="18">
+        <v>20</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <v>31</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="18">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="1"/>
+        <v>45.6</v>
+      </c>
+      <c r="F7" s="18">
+        <v>24</v>
+      </c>
+      <c r="G7" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
+        <v>26</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="18">
+        <f t="shared" si="0"/>
+        <v>46.6</v>
+      </c>
+      <c r="E8" s="18">
+        <f t="shared" si="1"/>
+        <v>53.2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>28</v>
+      </c>
+      <c r="G8" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <v>5</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="18">
+        <f t="shared" si="0"/>
+        <v>54.2</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" si="1"/>
+        <v>60.800000000000004</v>
+      </c>
+      <c r="F9" s="18">
+        <v>32</v>
+      </c>
+      <c r="G9" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>21</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="18">
+        <f t="shared" si="0"/>
+        <v>61.800000000000004</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" si="1"/>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F10" s="18">
+        <v>36</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
+        <v>2</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="18">
+        <f t="shared" si="0"/>
+        <v>69.400000000000006</v>
+      </c>
+      <c r="E11" s="18">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="F11" s="18">
+        <v>40</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>2</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="F12" s="18">
+        <v>44</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>8</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="F13" s="18">
+        <v>48</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>4</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="F14" s="18">
+        <v>52</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>3</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="F15" s="18">
+        <v>56</v>
+      </c>
+      <c r="G15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="F16" s="18">
+        <v>60</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>29</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="F17" s="18">
+        <v>64</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="24">
+        <v>8</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="F18" s="18">
+        <v>68</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
+        <v>8</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="F19" s="18">
+        <v>72</v>
+      </c>
+      <c r="G19" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
+        <v>7</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="F20" s="18">
+        <v>76</v>
+      </c>
+      <c r="G20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="24">
+        <v>2</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="24">
+        <v>11</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
+        <v>6</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="24">
+        <v>8</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>5</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="21">
+        <v>0</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="21">
+        <v>3</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
+        <v>7</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="21">
+        <v>2</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="21">
+        <v>5</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="21">
+        <v>9</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="21">
+        <v>0</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="21">
+        <v>4</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="21">
+        <v>15</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="23">
+        <v>6</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="23">
+        <v>25</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="23">
+        <v>3</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="24">
+        <v>76</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="24">
+        <v>36</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="24">
+        <v>53</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="24">
+        <v>3</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="24">
+        <v>4</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="24">
+        <v>2</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="24">
+        <v>71</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="24">
+        <v>4</v>
+      </c>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="24">
+        <v>16</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="24">
+        <v>3</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="24">
+        <v>16</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="24">
+        <v>0</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="24">
+        <v>8</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="24">
+        <v>8</v>
+      </c>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="24">
+        <v>8</v>
+      </c>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="24">
+        <v>22</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="24">
+        <v>26</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="24">
+        <v>7</v>
+      </c>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="24">
+        <v>5</v>
+      </c>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="24">
+        <v>3</v>
+      </c>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="24">
+        <v>7</v>
+      </c>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="24">
+        <v>2</v>
+      </c>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="24">
+        <v>6</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="24">
+        <v>6</v>
+      </c>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J24"/>
   <sheetViews>

</xml_diff>